<commit_message>
new function and fixing
</commit_message>
<xml_diff>
--- a/data-raw/Spreadsheet/GenBank_accessions_Randia_clade_RUBIACEAE.xlsx
+++ b/data-raw/Spreadsheet/GenBank_accessions_Randia_clade_RUBIACEAE.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domingoscardoso/Library/Mobile Documents/com~apple~CloudDocs/Publications_Phylogeny/catGenes/data-raw/Spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794BBCB6-CD85-2C4E-B724-D405595D0293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A401AEA6-C995-0E42-928E-2A319344726E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-6440" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$101</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="484">
   <si>
     <t>Species</t>
   </si>
@@ -1236,12 +1236,6 @@
     <t>AF183805</t>
   </si>
   <si>
-    <t>Jensen 4206A</t>
-  </si>
-  <si>
-    <t>AF183806</t>
-  </si>
-  <si>
     <t>Randia_chiapensis</t>
   </si>
   <si>
@@ -1284,9 +1278,6 @@
     <t>AF493461</t>
   </si>
   <si>
-    <t>AF493462</t>
-  </si>
-  <si>
     <t>Randia_longifolia</t>
   </si>
   <si>
@@ -1383,15 +1374,6 @@
     <t>AM182208</t>
   </si>
   <si>
-    <t>Randia_induta</t>
-  </si>
-  <si>
-    <t>Zedan</t>
-  </si>
-  <si>
-    <t>AM182206</t>
-  </si>
-  <si>
     <t>Randia_nelsonii</t>
   </si>
   <si>
@@ -1440,12 +1422,6 @@
     <t>Lopez 691</t>
   </si>
   <si>
-    <t>Lopez 691A</t>
-  </si>
-  <si>
-    <t>Randialaetevirens</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alberta_magna  </t>
   </si>
   <si>
@@ -1480,6 +1456,30 @@
   </si>
   <si>
     <t>Unvouchered</t>
+  </si>
+  <si>
+    <t>Plastome</t>
+  </si>
+  <si>
+    <t>MK577912</t>
+  </si>
+  <si>
+    <t>OR699446</t>
+  </si>
+  <si>
+    <t>KY348839</t>
+  </si>
+  <si>
+    <t>KY378662</t>
+  </si>
+  <si>
+    <t>KY378668</t>
+  </si>
+  <si>
+    <t>KY348836</t>
+  </si>
+  <si>
+    <t>NC_063574</t>
   </si>
 </sst>
 </file>
@@ -1765,11 +1765,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1782,10 +1784,11 @@
     <col min="6" max="6" width="11.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="11" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="12.5" style="2"/>
+    <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="12.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1810,10 +1813,13 @@
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I1" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>39</v>
@@ -1833,9 +1839,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>77</v>
@@ -1854,10 +1860,13 @@
       <c r="H3" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" s="4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>122</v>
@@ -1873,9 +1882,9 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1891,9 +1900,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>82</v>
@@ -1909,7 +1918,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>392</v>
       </c>
@@ -1931,9 +1940,9 @@
         <v>395</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>92</v>
@@ -1949,7 +1958,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>71</v>
       </c>
@@ -1971,7 +1980,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1993,7 +2002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -2017,12 +2026,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>240</v>
@@ -2043,7 +2052,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>246</v>
       </c>
@@ -2067,7 +2076,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>253</v>
       </c>
@@ -2089,7 +2098,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>365</v>
       </c>
@@ -2109,7 +2118,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>300</v>
       </c>
@@ -2130,10 +2139,13 @@
         <v>304</v>
       </c>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I16" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>58</v>
@@ -2153,9 +2165,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>89</v>
@@ -2170,8 +2182,11 @@
         <v>91</v>
       </c>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I18" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>106</v>
       </c>
@@ -2188,7 +2203,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>376</v>
       </c>
@@ -2208,7 +2223,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
@@ -2226,7 +2241,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>52</v>
       </c>
@@ -2248,7 +2263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
@@ -2268,7 +2283,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
@@ -2288,9 +2303,9 @@
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>100</v>
@@ -2304,7 +2319,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>102</v>
       </c>
@@ -2322,7 +2337,7 @@
       </c>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -2342,7 +2357,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>370</v>
       </c>
@@ -2364,7 +2379,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2386,7 +2401,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -2400,7 +2415,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
@@ -2422,7 +2437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
         <v>306</v>
       </c>
@@ -2439,6 +2454,9 @@
         <v>309</v>
       </c>
       <c r="H32" s="3"/>
+      <c r="I32" s="2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
@@ -2513,247 +2531,247 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>403</v>
+      <c r="A37" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="C38" s="3"/>
       <c r="D38" s="4" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>181</v>
-      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
-        <v>198</v>
+        <v>130</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C39" s="3"/>
+        <v>131</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="D39" s="4" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>136</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>170</v>
+      <c r="A41" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>447</v>
+      <c r="A42" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>153</v>
+      <c r="A43" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="B45" s="2" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>140</v>
+      <c r="D45" s="5" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>409</v>
-      </c>
+      <c r="A46" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D47" s="3"/>
+        <v>196</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>177</v>
-      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
+      <c r="A48" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>450</v>
+        <v>409</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>414</v>
+        <v>463</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>415</v>
@@ -2761,68 +2779,73 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>451</v>
+        <v>416</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>453</v>
+        <v>417</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>471</v>
+        <v>419</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>469</v>
+        <v>420</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>470</v>
+        <v>423</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>424</v>
-      </c>
+      <c r="A56" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
-        <v>425</v>
+        <v>448</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>427</v>
+        <v>449</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2837,859 +2860,830 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
+      <c r="A59" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
-        <v>454</v>
+        <v>434</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>456</v>
+        <v>435</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>433</v>
-      </c>
+      <c r="A61" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
-        <v>434</v>
+        <v>451</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>435</v>
+        <v>452</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>436</v>
+        <v>453</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>439</v>
-      </c>
+      <c r="A63" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="4" t="s">
-        <v>194</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G66" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>159</v>
+        <v>474</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D68" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="D70" s="5" t="s">
+      <c r="D69" s="5" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="3" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>149</v>
+        <v>226</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="E71" s="3"/>
-      <c r="F71" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D73" s="4"/>
+        <v>236</v>
+      </c>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>238</v>
+      </c>
       <c r="G73" s="3" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
-        <v>221</v>
+        <v>387</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>226</v>
+        <v>388</v>
       </c>
       <c r="C74" s="3"/>
-      <c r="D74" s="5" t="s">
-        <v>227</v>
-      </c>
+      <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-    </row>
-    <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F74" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
-        <v>228</v>
+        <v>63</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="E75" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="F75" s="3"/>
-      <c r="G75" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A76" s="3" t="s">
-        <v>234</v>
+      <c r="G75" s="3"/>
+      <c r="H75" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A76" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>236</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C76" s="3"/>
       <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="E76" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F76" s="3"/>
+      <c r="G76" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H76" s="3"/>
+      <c r="I76" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
-        <v>387</v>
+        <v>207</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C77" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3" t="s">
-        <v>390</v>
+        <v>211</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>391</v>
+        <v>212</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A78" s="3" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="E78" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A79" s="6" t="s">
-        <v>111</v>
+        <v>220</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A79" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="3" t="s">
-        <v>114</v>
+      <c r="E79" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="4" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="H79" s="3"/>
-    </row>
-    <row r="80" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="I79" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
-        <v>207</v>
+        <v>259</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>208</v>
+        <v>260</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>209</v>
+        <v>261</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3" t="s">
-        <v>211</v>
+        <v>262</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+        <v>263</v>
+      </c>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
-        <v>213</v>
+        <v>341</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>214</v>
+        <v>342</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>220</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
       <c r="F81" s="3" t="s">
-        <v>217</v>
+        <v>345</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>218</v>
+        <v>346</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
-        <v>85</v>
+        <v>264</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C82" s="3"/>
+        <v>265</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>266</v>
+      </c>
       <c r="D82" s="3"/>
-      <c r="E82" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F82" s="3"/>
-      <c r="G82" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="83" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
-        <v>259</v>
+        <v>310</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>260</v>
+        <v>311</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3" t="s">
-        <v>262</v>
+        <v>314</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="H83" s="3"/>
+        <v>315</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="84" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
-        <v>341</v>
+        <v>270</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>342</v>
+        <v>271</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>343</v>
+        <v>272</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>344</v>
-      </c>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
-        <v>264</v>
+        <v>321</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>265</v>
+        <v>322</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>266</v>
+        <v>323</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>267</v>
-      </c>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
+      <c r="F87" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="88" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
-        <v>321</v>
+        <v>359</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>322</v>
+        <v>360</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>323</v>
+        <v>361</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
+      <c r="F88" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="89" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>325</v>
+        <v>354</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>326</v>
+        <v>355</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3" t="s">
-        <v>328</v>
+        <v>357</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>329</v>
+        <v>358</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A90" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>276</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A90" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A93" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>461</v>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A93" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
-        <v>347</v>
+        <v>290</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>348</v>
+        <v>291</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>349</v>
+        <v>292</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>351</v>
+        <v>294</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>352</v>
+        <v>295</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
-        <v>330</v>
+        <v>290</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>333</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="C95" s="3"/>
+      <c r="D95" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F95" s="3"/>
+      <c r="G95" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
-        <v>336</v>
+        <v>290</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="C96" s="3"/>
+        <v>316</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>292</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C98" s="3"/>
-      <c r="D98" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="E98" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="F98" s="3"/>
-      <c r="G98" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="H98" s="3"/>
-    </row>
-    <row r="99" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A99" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="H99" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+        <v>285</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A99" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>280</v>
+        <v>115</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A101" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D101" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H100" s="3"/>
+      <c r="I100" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A101" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
       <c r="E101" s="3"/>
-      <c r="F101" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A102" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="G102" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="H102" s="5" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A103" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H103" s="3"/>
-    </row>
-    <row r="104" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A104" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C104" s="3"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="3"/>
-      <c r="F104" s="4" t="s">
+      <c r="F101" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G104" s="4" t="s">
+      <c r="G101" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="H104" s="3"/>
+      <c r="H101" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H76" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H104">
-    <sortCondition ref="A2:A104"/>
+  <autoFilter ref="A1:I101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H101">
+    <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>